<commit_message>
Added CSV file for constants
</commit_message>
<xml_diff>
--- a/Drag_Constants.xlsx
+++ b/Drag_Constants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prana\Desktop\1 - College\4 Club Work\Team Anant\ADCS\Orbit-Propagator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5CCDA3-E5A4-4625-8567-90822525B7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41424E-8153-4D9A-985C-BBBC742CDD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9D9F116A-68EF-41E1-B9B6-39BA499BABF9}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>po (kg/m3 )</t>
   </si>
   <si>
-    <t>H (km)</t>
+    <t>H (m)</t>
   </si>
 </sst>
 </file>
@@ -421,13 +421,13 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
@@ -452,392 +452,392 @@
         <v>1.2250000000000001</v>
       </c>
       <c r="C2">
-        <v>8.44</v>
+        <v>8440</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="B3" s="1">
         <v>3.8989999999999997E-2</v>
       </c>
       <c r="C3">
-        <v>6.49</v>
+        <v>6490</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="B4" s="1">
         <v>1.7739999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>6.75</v>
+        <v>6750</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="B5" s="1">
         <v>8.2789999999999999E-3</v>
       </c>
       <c r="C5">
-        <v>7.07</v>
+        <v>7070</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>40</v>
+        <v>40000</v>
       </c>
       <c r="B6" s="1">
         <v>3.9719999999999998E-3</v>
       </c>
       <c r="C6">
-        <v>7.47</v>
+        <v>7470</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>45</v>
+        <v>45000</v>
       </c>
       <c r="B7" s="1">
         <v>1.9949999999999998E-3</v>
       </c>
       <c r="C7">
-        <v>7.83</v>
+        <v>7830</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="B8" s="1">
         <v>1.057E-3</v>
       </c>
       <c r="C8">
-        <v>7.95</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>55</v>
+        <v>55000</v>
       </c>
       <c r="B9" s="1">
         <v>5.821E-4</v>
       </c>
       <c r="C9">
-        <v>7.73</v>
+        <v>7730</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>60</v>
+        <v>60000</v>
       </c>
       <c r="B10" s="1">
         <v>3.2059999999999999E-4</v>
       </c>
       <c r="C10">
-        <v>7.29</v>
+        <v>7290</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>65</v>
+        <v>65000</v>
       </c>
       <c r="B11" s="1">
         <v>1.718E-4</v>
       </c>
       <c r="C11">
-        <v>6.81</v>
+        <v>6810</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>70</v>
+        <v>70000</v>
       </c>
       <c r="B12" s="1">
         <v>8.7700000000000004E-5</v>
       </c>
       <c r="C12">
-        <v>6.33</v>
+        <v>6330</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="B13" s="1">
         <v>4.1780000000000003E-5</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>80</v>
+        <v>80000</v>
       </c>
       <c r="B14" s="1">
         <v>1.9049999999999999E-5</v>
       </c>
       <c r="C14">
-        <v>5.7</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>85</v>
+        <v>85000</v>
       </c>
       <c r="B15" s="1">
         <v>8.337E-6</v>
       </c>
       <c r="C15">
-        <v>5.41</v>
+        <v>5410</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>90</v>
+        <v>90000</v>
       </c>
       <c r="B16" s="1">
         <v>3.3960000000000002E-6</v>
       </c>
       <c r="C16">
-        <v>5.38</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>95</v>
+        <v>95000</v>
       </c>
       <c r="B17" s="1">
         <v>1.3430000000000001E-6</v>
       </c>
       <c r="C17">
-        <v>5.74</v>
+        <v>5740</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="B18" s="1">
         <v>5.2969999999999999E-7</v>
       </c>
       <c r="C18">
-        <v>6.15</v>
+        <v>6150</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>110</v>
+        <v>110000</v>
       </c>
       <c r="B19" s="1">
         <v>9.6610000000000003E-8</v>
       </c>
       <c r="C19">
-        <v>8.06</v>
+        <v>8060.0000000000009</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>120</v>
+        <v>120000</v>
       </c>
       <c r="B20" s="1">
         <v>2.4380000000000001E-8</v>
       </c>
       <c r="C20">
-        <v>11.6</v>
+        <v>11600</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>130</v>
+        <v>130000</v>
       </c>
       <c r="B21" s="1">
         <v>8.4840000000000001E-9</v>
       </c>
       <c r="C21">
-        <v>16.100000000000001</v>
+        <v>16100.000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>140</v>
+        <v>140000</v>
       </c>
       <c r="B22" s="1">
         <v>3.8449999999999999E-9</v>
       </c>
       <c r="C22">
-        <v>20.6</v>
+        <v>20600</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>150</v>
+        <v>150000</v>
       </c>
       <c r="B23" s="1">
         <v>2.0700000000000001E-9</v>
       </c>
       <c r="C23">
-        <v>24.6</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>160</v>
+        <v>160000</v>
       </c>
       <c r="B24" s="1">
         <v>1.2239999999999999E-9</v>
       </c>
       <c r="C24">
-        <v>26.3</v>
+        <v>26300</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>180</v>
+        <v>180000</v>
       </c>
       <c r="B25" s="1">
         <v>5.4639999999999999E-10</v>
       </c>
       <c r="C25">
-        <v>33.200000000000003</v>
+        <v>33200</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>200</v>
+        <v>200000</v>
       </c>
       <c r="B26" s="1">
         <v>2.7889999999999999E-10</v>
       </c>
       <c r="C26">
-        <v>38.5</v>
+        <v>38500</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>250</v>
+        <v>250000</v>
       </c>
       <c r="B27" s="1">
         <v>7.2480000000000005E-11</v>
       </c>
       <c r="C27">
-        <v>46.9</v>
+        <v>46900</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="B28" s="1">
         <v>2.4180000000000001E-11</v>
       </c>
       <c r="C28">
-        <v>52.5</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>350</v>
+        <v>350000</v>
       </c>
       <c r="B29" s="1">
         <v>9.1579999999999995E-12</v>
       </c>
       <c r="C29">
-        <v>56.4</v>
+        <v>56400</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>400</v>
+        <v>400000</v>
       </c>
       <c r="B30" s="1">
         <v>3.7250000000000004E-12</v>
       </c>
       <c r="C30">
-        <v>59.4</v>
+        <v>59400</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>450</v>
+        <v>450000</v>
       </c>
       <c r="B31" s="1">
         <v>1.585E-12</v>
       </c>
       <c r="C31">
-        <v>62.2</v>
+        <v>62200</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>500</v>
+        <v>500000</v>
       </c>
       <c r="B32" s="1">
         <v>6.9670000000000005E-13</v>
       </c>
       <c r="C32">
-        <v>65.8</v>
+        <v>65800</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>600</v>
+        <v>600000</v>
       </c>
       <c r="B33" s="1">
         <v>1.4539999999999999E-13</v>
       </c>
       <c r="C33">
-        <v>79</v>
+        <v>79000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>700</v>
+        <v>700000</v>
       </c>
       <c r="B34" s="1">
         <v>3.6139999999999998E-14</v>
       </c>
       <c r="C34">
-        <v>109</v>
+        <v>109000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>800</v>
+        <v>800000</v>
       </c>
       <c r="B35" s="1">
         <v>1.17E-14</v>
       </c>
       <c r="C35">
-        <v>164</v>
+        <v>164000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>900</v>
+        <v>900000</v>
       </c>
       <c r="B36" s="1">
         <v>5.2449999999999998E-15</v>
       </c>
       <c r="C36">
-        <v>225</v>
+        <v>225000</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="B37" s="1">
         <v>3.019E-15</v>
       </c>
       <c r="C37">
-        <v>268</v>
+        <v>268000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>